<commit_message>
added graph for 3 year average of expenditures
</commit_message>
<xml_diff>
--- a/graphs/RUD_na_obyvatele_analyza_2024.xlsx
+++ b/graphs/RUD_na_obyvatele_analyza_2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,6 +461,11 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Index (ČR=100)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Podíl na RUD ČR (%)</t>
         </is>
       </c>
@@ -484,6 +489,9 @@
         <v>249.5</v>
       </c>
       <c r="F2" t="n">
+        <v>249</v>
+      </c>
+      <c r="G2" t="n">
         <v>31.8</v>
       </c>
     </row>
@@ -506,6 +514,9 @@
         <v>94.8</v>
       </c>
       <c r="F3" t="n">
+        <v>95</v>
+      </c>
+      <c r="G3" t="n">
         <v>10.7</v>
       </c>
     </row>
@@ -528,6 +539,9 @@
         <v>92.3</v>
       </c>
       <c r="F4" t="n">
+        <v>92</v>
+      </c>
+      <c r="G4" t="n">
         <v>5.2</v>
       </c>
     </row>
@@ -550,6 +564,9 @@
         <v>91</v>
       </c>
       <c r="F5" t="n">
+        <v>91</v>
+      </c>
+      <c r="G5" t="n">
         <v>9.9</v>
       </c>
     </row>
@@ -572,6 +589,9 @@
         <v>73.5</v>
       </c>
       <c r="F6" t="n">
+        <v>73</v>
+      </c>
+      <c r="G6" t="n">
         <v>5.5</v>
       </c>
     </row>
@@ -594,6 +614,9 @@
         <v>73.3</v>
       </c>
       <c r="F7" t="n">
+        <v>73</v>
+      </c>
+      <c r="G7" t="n">
         <v>3</v>
       </c>
     </row>
@@ -616,6 +639,9 @@
         <v>72.09999999999999</v>
       </c>
       <c r="F8" t="n">
+        <v>72</v>
+      </c>
+      <c r="G8" t="n">
         <v>4.2</v>
       </c>
     </row>
@@ -638,6 +664,9 @@
         <v>71.7</v>
       </c>
       <c r="F9" t="n">
+        <v>72</v>
+      </c>
+      <c r="G9" t="n">
         <v>1.9</v>
       </c>
     </row>
@@ -660,6 +689,9 @@
         <v>71.59999999999999</v>
       </c>
       <c r="F10" t="n">
+        <v>72</v>
+      </c>
+      <c r="G10" t="n">
         <v>3.7</v>
       </c>
     </row>
@@ -682,6 +714,9 @@
         <v>71.40000000000001</v>
       </c>
       <c r="F11" t="n">
+        <v>71</v>
+      </c>
+      <c r="G11" t="n">
         <v>3.5</v>
       </c>
     </row>
@@ -704,6 +739,9 @@
         <v>71.40000000000001</v>
       </c>
       <c r="F12" t="n">
+        <v>71</v>
+      </c>
+      <c r="G12" t="n">
         <v>3.8</v>
       </c>
     </row>
@@ -726,6 +764,9 @@
         <v>71.3</v>
       </c>
       <c r="F13" t="n">
+        <v>71</v>
+      </c>
+      <c r="G13" t="n">
         <v>4.3</v>
       </c>
     </row>
@@ -748,6 +789,9 @@
         <v>70.2</v>
       </c>
       <c r="F14" t="n">
+        <v>70</v>
+      </c>
+      <c r="G14" t="n">
         <v>3.3</v>
       </c>
     </row>
@@ -770,6 +814,9 @@
         <v>69.5</v>
       </c>
       <c r="F15" t="n">
+        <v>69</v>
+      </c>
+      <c r="G15" t="n">
         <v>9.300000000000001</v>
       </c>
     </row>

</xml_diff>